<commit_message>
weather update last: sea lb
</commit_message>
<xml_diff>
--- a/Weather-Bigdata-Contest/기상데이터_컬럼.xlsx
+++ b/Weather-Bigdata-Contest/기상데이터_컬럼.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B0113\weather_bd_contest_workspace\Weather-Bigdata-Contest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2396A9E-4842-4AC9-B68C-C7159F0EFEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088601FC-4999-4706-A6C4-93753317361B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="899" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1329,7 +1329,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>